<commit_message>
Finished all text, tested for stability but not typos
</commit_message>
<xml_diff>
--- a/navigationGenerator.xlsx
+++ b/navigationGenerator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\CuddlyCthulhuCreatives\VideoGames\FetchQuest\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\CuddlyCthulhuCreatives\VideoGames\FetchQuest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2528F90B-77D8-442E-8A3C-565C56DF9631}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE1CE1F-6126-465F-A353-9B41480BF489}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="20400" windowHeight="7530" xr2:uid="{40A337B8-7C11-4573-ACCA-463B2E1C0977}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20400" windowHeight="7530" xr2:uid="{40A337B8-7C11-4573-ACCA-463B2E1C0977}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,31 +33,31 @@
     <t>"NOTHING"</t>
   </si>
   <si>
-    <t>"Stick"</t>
+    <t>"First Aid Kit"</t>
   </si>
   <si>
-    <t>"Dog Food"</t>
+    <t>"Take a look in the kitchen"</t>
   </si>
   <si>
-    <t>"Leave the wood"</t>
+    <t>"emptyHouseKitchen"</t>
   </si>
   <si>
-    <t>"Go to the den"</t>
+    <t>"emptyHouseBasement"</t>
   </si>
   <si>
-    <t>"exterior"</t>
+    <t>"emptyHouseBedroom"</t>
   </si>
   <si>
-    <t>"woodDen"</t>
+    <t>emptyHouseInterior</t>
   </si>
   <si>
-    <t>"woodExplore"</t>
+    <t>"Check out the basement"</t>
   </si>
   <si>
-    <t>woodCollar</t>
+    <t>"Head up to the bedroom"</t>
   </si>
   <si>
-    <t>"Explore the wood"</t>
+    <t>"missingAidKit"</t>
   </si>
 </sst>
 </file>
@@ -436,12 +436,12 @@
   <dimension ref="A2:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D38"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="81.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" customWidth="1"/>
   </cols>
@@ -449,7 +449,7 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D2" t="str">
         <f>"//--"&amp;Table1[section]&amp;"--//"</f>
-        <v>//--woodCollar--//</v>
+        <v>//--emptyHouseInterior--//</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
@@ -460,18 +460,18 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="C3" s="1" t="str">
         <f>""""&amp;Table1[section]&amp;"Choices"""</f>
-        <v>"woodCollarChoices"</v>
+        <v>"emptyHouseInteriorChoices"</v>
       </c>
       <c r="D3" t="str">
         <f>"ds_grid_set(global.navigation, "&amp;A3&amp;", "&amp;B3&amp;", "&amp;C3&amp;" );"</f>
-        <v>ds_grid_set(global.navigation, 0, 48, "woodCollarChoices" );</v>
+        <v>ds_grid_set(global.navigation, 0, 128, "emptyHouseInteriorChoices" );</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -479,14 +479,14 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ref="D4:D38" si="0">"ds_grid_set(global.navigation, "&amp;A4&amp;", "&amp;B4&amp;", "&amp;C4&amp;" );"</f>
-        <v>ds_grid_set(global.navigation, 1, 48, "Go to the den" );</v>
+        <v>ds_grid_set(global.navigation, 1, 128, "Take a look in the kitchen" );</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -494,14 +494,14 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 2, 48, "Explore the wood" );</v>
+        <v>ds_grid_set(global.navigation, 2, 128, "Check out the basement" );</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -509,14 +509,14 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 3, 48, "Leave the wood" );</v>
+        <v>ds_grid_set(global.navigation, 3, 128, "Head up to the bedroom" );</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -524,14 +524,14 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 4, 48, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 4, 128, "NOTHING" );</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -539,14 +539,14 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 5, 48, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 5, 128, "NOTHING" );</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -554,15 +554,15 @@
         <v>0</v>
       </c>
       <c r="B9">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>""""&amp;Table1[section]&amp;"Targets"""</f>
-        <v>"woodCollarTargets"</v>
+        <v>"emptyHouseInteriorTargets"</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 0, 49, "woodCollarTargets" );</v>
+        <v>ds_grid_set(global.navigation, 0, 129, "emptyHouseInteriorTargets" );</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -570,14 +570,14 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 1, 49, "woodDen" );</v>
+        <v>ds_grid_set(global.navigation, 1, 129, "emptyHouseKitchen" );</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -585,14 +585,14 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 2, 49, "woodExplore" );</v>
+        <v>ds_grid_set(global.navigation, 2, 129, "emptyHouseBasement" );</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -600,14 +600,14 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 3, 49, "exterior" );</v>
+        <v>ds_grid_set(global.navigation, 3, 129, "emptyHouseBedroom" );</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -615,14 +615,14 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 4, 49, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 4, 129, "NOTHING" );</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -630,14 +630,14 @@
         <v>5</v>
       </c>
       <c r="B14">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 5, 49, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 5, 129, "NOTHING" );</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -645,15 +645,15 @@
         <v>0</v>
       </c>
       <c r="B15">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>""""&amp;Table1[section]&amp;"InventoryGet"""</f>
-        <v>"woodCollarInventoryGet"</v>
+        <v>"emptyHouseInteriorInventoryGet"</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 0, 50, "woodCollarInventoryGet" );</v>
+        <v>ds_grid_set(global.navigation, 0, 130, "emptyHouseInteriorInventoryGet" );</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -661,14 +661,14 @@
         <v>1</v>
       </c>
       <c r="B16">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 1, 50, "Dog Food" );</v>
+        <v>ds_grid_set(global.navigation, 1, 130, "NOTHING" );</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -676,14 +676,14 @@
         <v>2</v>
       </c>
       <c r="B17">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 2, 50, "Stick" );</v>
+        <v>ds_grid_set(global.navigation, 2, 130, "NOTHING" );</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,14 +691,14 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 3, 50, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 3, 130, "NOTHING" );</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -706,14 +706,14 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 4, 50, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 4, 130, "NOTHING" );</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -721,14 +721,14 @@
         <v>5</v>
       </c>
       <c r="B20">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 5, 50, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 5, 130, "NOTHING" );</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -736,15 +736,15 @@
         <v>0</v>
       </c>
       <c r="B21">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="C21" s="1" t="str">
         <f>""""&amp;Table1[section]&amp;"InventoryNeed"""</f>
-        <v>"woodCollarInventoryNeed"</v>
+        <v>"emptyHouseInteriorInventoryNeed"</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 0, 51, "woodCollarInventoryNeed" );</v>
+        <v>ds_grid_set(global.navigation, 0, 131, "emptyHouseInteriorInventoryNeed" );</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -752,14 +752,14 @@
         <v>1</v>
       </c>
       <c r="B22">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 1, 51, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 1, 131, "NOTHING" );</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -767,14 +767,14 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 2, 51, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 2, 131, "First Aid Kit" );</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -782,14 +782,14 @@
         <v>3</v>
       </c>
       <c r="B24">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 3, 51, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 3, 131, "NOTHING" );</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -797,14 +797,14 @@
         <v>4</v>
       </c>
       <c r="B25">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 4, 51, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 4, 131, "NOTHING" );</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -812,14 +812,14 @@
         <v>5</v>
       </c>
       <c r="B26">
-        <v>51</v>
+        <v>131</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 5, 51, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 5, 131, "NOTHING" );</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -827,15 +827,15 @@
         <v>0</v>
       </c>
       <c r="B27">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C27" s="1" t="str">
         <f>""""&amp;Table1[section]&amp;"InventoryMissingTarget"""</f>
-        <v>"woodCollarInventoryMissingTarget"</v>
+        <v>"emptyHouseInteriorInventoryMissingTarget"</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 0, 52, "woodCollarInventoryMissingTarget" );</v>
+        <v>ds_grid_set(global.navigation, 0, 132, "emptyHouseInteriorInventoryMissingTarget" );</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -843,14 +843,14 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 1, 52, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 1, 132, "NOTHING" );</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -858,14 +858,14 @@
         <v>2</v>
       </c>
       <c r="B29">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 2, 52, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 2, 132, "missingAidKit" );</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -873,14 +873,14 @@
         <v>3</v>
       </c>
       <c r="B30">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 3, 52, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 3, 132, "NOTHING" );</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -888,14 +888,14 @@
         <v>4</v>
       </c>
       <c r="B31">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 4, 52, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 4, 132, "NOTHING" );</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -903,14 +903,14 @@
         <v>5</v>
       </c>
       <c r="B32">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 5, 52, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 5, 132, "NOTHING" );</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -918,15 +918,15 @@
         <v>0</v>
       </c>
       <c r="B33">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="C33" s="1" t="str">
         <f>""""&amp;Table1[section]&amp;"InventoryDestroy"""</f>
-        <v>"woodCollarInventoryDestroy"</v>
+        <v>"emptyHouseInteriorInventoryDestroy"</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 0, 53, "woodCollarInventoryDestroy" );</v>
+        <v>ds_grid_set(global.navigation, 0, 133, "emptyHouseInteriorInventoryDestroy" );</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -934,14 +934,14 @@
         <v>1</v>
       </c>
       <c r="B34">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 1, 53, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 1, 133, "NOTHING" );</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -949,14 +949,14 @@
         <v>2</v>
       </c>
       <c r="B35">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 2, 53, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 2, 133, "First Aid Kit" );</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -964,14 +964,14 @@
         <v>3</v>
       </c>
       <c r="B36">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 3, 53, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 3, 133, "NOTHING" );</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -979,14 +979,14 @@
         <v>4</v>
       </c>
       <c r="B37">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 4, 53, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 4, 133, "NOTHING" );</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -994,14 +994,14 @@
         <v>5</v>
       </c>
       <c r="B38">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v>ds_grid_set(global.navigation, 5, 53, "NOTHING" );</v>
+        <v>ds_grid_set(global.navigation, 5, 133, "NOTHING" );</v>
       </c>
     </row>
   </sheetData>

</xml_diff>